<commit_message>
update for final of tds
</commit_message>
<xml_diff>
--- a/elo/fantasy_scores.xlsx
+++ b/elo/fantasy_scores.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syverjohansen/ski/elo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D1547A-8CA5-C549-BBE6-FB115DBC5B9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFD1D9C-1C53-5E45-AC51-B2A6579F4641}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21940" yWindow="5920" windowWidth="20520" windowHeight="15080" xr2:uid="{B0998D18-19B6-A845-A65E-EF44614B0821}"/>
+    <workbookView xWindow="16580" yWindow="980" windowWidth="20520" windowHeight="15080" xr2:uid="{B0998D18-19B6-A845-A65E-EF44614B0821}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>me</t>
   </si>
@@ -49,6 +49,12 @@
   </si>
   <si>
     <t>CP</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>SC</t>
   </si>
 </sst>
 </file>
@@ -400,10 +406,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B2AAD67-6582-B144-BA35-366945DC59BE}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,65 +438,152 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>20200105</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2">
-        <f>(50+46+43+34+32+30+15+13)+(50+46+40+30+37+24+20+11)</f>
-        <v>521</v>
+        <f t="shared" ref="C2:H2" si="0">SUM(C3:C999999)</f>
+        <v>2012</v>
       </c>
       <c r="D2">
-        <f>(30+43+37+13+32+46+11+5)+(10+43+50+46+37+0+3+0)</f>
-        <v>406</v>
+        <f t="shared" si="0"/>
+        <v>1720</v>
       </c>
       <c r="E2">
-        <f>(30+43+13+32+9+46+11+5)+(10+43+50+30+37+20+0+3)</f>
-        <v>382</v>
+        <f t="shared" si="0"/>
+        <v>1841</v>
       </c>
       <c r="F2">
-        <f>(50+30+13+32+46+15+34+5)+(43+50+40+30+20+24+14)</f>
-        <v>446</v>
+        <f t="shared" si="0"/>
+        <v>1923</v>
       </c>
       <c r="G2">
-        <f>(50+30+13+32+46+15+34+5)+(43+50+40+30+20+24+14)</f>
-        <v>446</v>
+        <f t="shared" si="0"/>
+        <v>1923</v>
       </c>
       <c r="H2">
-        <v>608</v>
+        <f t="shared" si="0"/>
+        <v>2450</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>20200106</v>
+        <v>20210105</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <f>(50+46+43+34+32+30+15+13)+(50+46+40+30+37+24+20+11)</f>
+        <v>521</v>
+      </c>
+      <c r="D3">
+        <f>(30+43+37+13+32+46+11+5)+(10+43+50+46+37+0+3+0)</f>
+        <v>406</v>
+      </c>
+      <c r="E3">
+        <f>(30+43+13+32+9+46+11+5)+(10+43+50+30+37+20+0+3)</f>
+        <v>382</v>
+      </c>
+      <c r="F3">
+        <f>(50+30+13+32+46+15+34+5)+(43+50+40+30+20+24+14)</f>
+        <v>446</v>
+      </c>
+      <c r="G3">
+        <f>(50+30+13+32+46+15+34+5)+(43+50+40+30+20+24+14)</f>
+        <v>446</v>
+      </c>
+      <c r="H3">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>20210106</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C3">
+      <c r="C4">
         <f>(46+40+34+30+43+37+32+9)+(46+37+22+6+43+28+20+2)</f>
         <v>475</v>
       </c>
-      <c r="D3">
+      <c r="D4">
         <f>(50+46+30+40+43+32+34+24)+(50+46+43+40+37+28+32+13)</f>
         <v>588</v>
       </c>
-      <c r="E3">
+      <c r="E4">
         <f>(37+46+30+40+32+34+43+24)+(50+46+43+40+37+34+22+13)</f>
         <v>571</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <f>(37+46+30+14+40+43+34+32)+(50+46+43+40+37+34+22+32)</f>
         <v>580</v>
       </c>
-      <c r="G3">
+      <c r="G4">
         <f>(37+46+30+14+40+43+34+32)+(50+46+43+40+37+34+22+32)</f>
         <v>580</v>
       </c>
-      <c r="H3">
+      <c r="H4">
         <v>604</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>20210108</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <f>(50+40+32+11+43+37+26+7)+(46+43+34+32+30+28+26+16)</f>
+        <v>501</v>
+      </c>
+      <c r="D5">
+        <f>(32+37+22+7+46+11+0+4)+(28+50+0+30+34+20+15+14)</f>
+        <v>350</v>
+      </c>
+      <c r="E5">
+        <f>(32+37+4+22+7+46+11+0)+(43+28+0+30+40+34+46+16)</f>
+        <v>396</v>
+      </c>
+      <c r="F5">
+        <f>(32+37+22+7+46+11+0+0)+(50+43+28+30+40+34+46+32)</f>
+        <v>458</v>
+      </c>
+      <c r="G5">
+        <v>458</v>
+      </c>
+      <c r="H5">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>20210109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <f>(50+46+40+34+28+24+13+2)+(50+46+40+34+32+30+28+18)</f>
+        <v>515</v>
+      </c>
+      <c r="D6">
+        <f>(24+20+34+0+18+14+0+16)+(40+26+22+30+34+50+16+32)</f>
+        <v>376</v>
+      </c>
+      <c r="E6">
+        <f>(40+46+24+2+34+50+37+9)+(26+28+24+34+10+50+46+32)</f>
+        <v>492</v>
+      </c>
+      <c r="F6">
+        <f>(40+46+1+18+16+50+37+13)+(40+26+28+30+34+10+32+18)</f>
+        <v>439</v>
+      </c>
+      <c r="G6">
+        <f>(40+46+1+18+16+50+37+13)+(40+26+28+30+34+10+32+18)</f>
+        <v>439</v>
+      </c>
+      <c r="H6">
+        <v>618</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
included stuff for relays
</commit_message>
<xml_diff>
--- a/elo/fantasy_scores.xlsx
+++ b/elo/fantasy_scores.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syverjohansen/ski/elo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FFD1D9C-1C53-5E45-AC51-B2A6579F4641}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41781B45-D91D-BC47-9EFF-9CE8F7422D1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16580" yWindow="980" windowWidth="20520" windowHeight="15080" xr2:uid="{B0998D18-19B6-A845-A65E-EF44614B0821}"/>
+    <workbookView xWindow="14400" yWindow="900" windowWidth="20520" windowHeight="15080" xr2:uid="{B0998D18-19B6-A845-A65E-EF44614B0821}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>me</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>SC</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>TdS</t>
   </si>
 </sst>
 </file>
@@ -406,13 +412,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B2AAD67-6582-B144-BA35-366945DC59BE}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,27 +446,27 @@
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C2">
         <f t="shared" ref="C2:H2" si="0">SUM(C3:C999999)</f>
-        <v>2012</v>
+        <v>5872</v>
       </c>
       <c r="D2">
         <f t="shared" si="0"/>
-        <v>1720</v>
+        <v>5286</v>
       </c>
       <c r="E2">
         <f t="shared" si="0"/>
-        <v>1841</v>
+        <v>5612</v>
       </c>
       <c r="F2">
         <f t="shared" si="0"/>
-        <v>1923</v>
+        <v>5756</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
-        <v>1923</v>
+        <v>5756</v>
       </c>
       <c r="H2">
         <f t="shared" si="0"/>
-        <v>2450</v>
+        <v>6450</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -584,6 +590,68 @@
       </c>
       <c r="H6">
         <v>618</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>20200110</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <f>(50+46+40+37+32+26+14+6)+(50+46+43+40+34+30+22+20)</f>
+        <v>536</v>
+      </c>
+      <c r="D7">
+        <f>(37+34+22+14+40+0+50+43)+(24+46+32+40+22+0+0+6)</f>
+        <v>410</v>
+      </c>
+      <c r="E7">
+        <f>(37+34+22+14+40+0+50+43)+(24+50+46+20+22+30+34+13)</f>
+        <v>479</v>
+      </c>
+      <c r="F7">
+        <f>(46+37+14+40+50+26+43+0)+(50+46+40+20+22+30+34+43)</f>
+        <v>541</v>
+      </c>
+      <c r="G7">
+        <f>(46+37+14+40+50+26+43+0)+(50+46+40+20+22+30+34+43)</f>
+        <v>541</v>
+      </c>
+      <c r="H7">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>20200110</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8">
+        <f>(400+320+240+200+180+160+128+116)+(400+320+200+180+160+128+104+88)</f>
+        <v>3324</v>
+      </c>
+      <c r="D8">
+        <f>(400+200+180+128+160+240+116+320)+(144+400+320+180+72+128+88+80)</f>
+        <v>3156</v>
+      </c>
+      <c r="E8">
+        <f>(400+200+180+128+160+116+240+320)+(400+160+320+200+180+72+128+88)</f>
+        <v>3292</v>
+      </c>
+      <c r="F8">
+        <f>(400+200+180+128+240+116+160+320)+(400+160+320+200+180+72+128+88)</f>
+        <v>3292</v>
+      </c>
+      <c r="G8">
+        <f>(400+200+180+128+240+116+160+320)+(400+160+320+200+180+72+128+88)</f>
+        <v>3292</v>
+      </c>
+      <c r="H8">
+        <v>3380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>